<commit_message>
v2 PCB mostly done, DRC and final check remaining
</commit_message>
<xml_diff>
--- a/Documents/ComponentPowerRequirements.xlsx
+++ b/Documents/ComponentPowerRequirements.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9540" windowHeight="3345" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="ComponentPowerRequirements" sheetId="1" r:id="rId1"/>
+    <sheet name="v1" sheetId="1" r:id="rId1"/>
+    <sheet name="v2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="101">
   <si>
     <t>IC</t>
   </si>
@@ -277,6 +278,51 @@
   </si>
   <si>
     <t>TCR3UM18A,LF</t>
+  </si>
+  <si>
+    <t>TPA3250</t>
+  </si>
+  <si>
+    <t>38V</t>
+  </si>
+  <si>
+    <t>36V</t>
+  </si>
+  <si>
+    <t>10.8V</t>
+  </si>
+  <si>
+    <t>13.2V</t>
+  </si>
+  <si>
+    <t>65mA</t>
+  </si>
+  <si>
+    <t>nRF5340</t>
+  </si>
+  <si>
+    <t>7mA</t>
+  </si>
+  <si>
+    <t>5V to 3.3V nRF5340 DC/DC</t>
+  </si>
+  <si>
+    <t>Fan</t>
+  </si>
+  <si>
+    <t>F251R-12LLC</t>
+  </si>
+  <si>
+    <t>10.2V</t>
+  </si>
+  <si>
+    <t>13.8V</t>
+  </si>
+  <si>
+    <t>40mA</t>
+  </si>
+  <si>
+    <t>Power Supply Fan Port</t>
   </si>
 </sst>
 </file>
@@ -419,7 +465,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -632,6 +678,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -950,7 +1002,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -988,151 +1040,187 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1458,7 +1546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -1510,356 +1598,356 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="19" t="s">
+      <c r="J2" s="17" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="26" t="s">
+      <c r="A3" s="67"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="H3" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="26" t="s">
+      <c r="I3" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="27" t="s">
+      <c r="J3" s="25" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="23" t="s">
+      <c r="J4" s="21" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="24" t="s">
+      <c r="A5" s="67"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="24" t="s">
+      <c r="G5" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="H5" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="24" t="s">
+      <c r="I5" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="25" t="s">
+      <c r="J5" s="23" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="24" t="s">
+      <c r="A6" s="67"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="H6" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="24" t="s">
+      <c r="I6" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="25" t="s">
+      <c r="J6" s="23" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="24" t="s">
+      <c r="A7" s="67"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="24" t="s">
+      <c r="G7" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="24" t="s">
+      <c r="H7" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="I7" s="24" t="s">
+      <c r="I7" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="J7" s="25" t="s">
+      <c r="J7" s="23" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="63" t="s">
         <v>47</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="H8" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="J8" s="21" t="s">
+      <c r="J8" s="19" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
+      <c r="A9" s="67"/>
       <c r="B9" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="28" t="s">
+      <c r="F9" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="G9" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="28" t="s">
+      <c r="H9" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="28" t="s">
+      <c r="I9" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="J9" s="29" t="s">
+      <c r="J9" s="27" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="60" t="s">
+      <c r="C10" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="60" t="s">
+      <c r="D10" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="E10" s="60" t="s">
+      <c r="E10" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="60" t="s">
+      <c r="F10" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="G10" s="60" t="s">
+      <c r="G10" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="H10" s="60" t="s">
+      <c r="H10" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="I10" s="60" t="s">
+      <c r="I10" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="61" t="s">
+      <c r="J10" s="54" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="30" t="s">
+      <c r="A11" s="67"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="30" t="s">
+      <c r="F11" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="30" t="s">
+      <c r="G11" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="H11" s="30" t="s">
+      <c r="H11" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="I11" s="30" t="s">
+      <c r="I11" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="J11" s="31" t="s">
+      <c r="J11" s="29" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="58" t="s">
+      <c r="A12" s="67"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="58" t="s">
+      <c r="D12" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="58" t="s">
+      <c r="E12" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="58" t="s">
+      <c r="F12" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="G12" s="58" t="s">
+      <c r="G12" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="H12" s="58" t="s">
+      <c r="H12" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="I12" s="58" t="s">
+      <c r="I12" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="J12" s="59" t="s">
+      <c r="J12" s="52" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="16" t="s">
+      <c r="A13" s="62"/>
+      <c r="B13" s="66"/>
+      <c r="C13" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="I13" s="16" t="s">
+      <c r="I13" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="J13" s="17" t="s">
+      <c r="J13" s="15" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1878,30 +1966,30 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="52" t="s">
+      <c r="A17" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="53" t="s">
+      <c r="B17" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="53" t="s">
+      <c r="C17" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="54" t="s">
+      <c r="D17" s="47" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="49" t="s">
+      <c r="A18" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="B18" s="50" t="s">
+      <c r="B18" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="50" t="s">
+      <c r="C18" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="51" t="s">
+      <c r="D18" s="44" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1915,119 +2003,119 @@
       <c r="C20" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="35" t="s">
+      <c r="D20" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="36"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="58"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="37" t="s">
+      <c r="A21" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="38" t="s">
+      <c r="B21" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="39" t="s">
+      <c r="C21" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="D21" s="43" t="s">
+      <c r="D21" s="61" t="s">
         <v>77</v>
       </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="33"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="59"/>
+      <c r="H21" s="60"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="40" t="s">
+      <c r="A22" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="41" t="s">
+      <c r="B22" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="42" t="s">
+      <c r="C22" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="43" t="s">
+      <c r="D22" s="62"/>
+      <c r="E22" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="33"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="59"/>
+      <c r="H22" s="60"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="46" t="s">
+      <c r="A23" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="47" t="s">
+      <c r="B23" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="48" t="s">
+      <c r="C23" s="41" t="s">
         <v>71</v>
       </c>
       <c r="D23" s="5"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="10" t="s">
+      <c r="E23" s="62"/>
+      <c r="F23" s="63" t="s">
         <v>76</v>
       </c>
-      <c r="G23" s="43" t="s">
+      <c r="G23" s="61" t="s">
         <v>78</v>
       </c>
       <c r="H23" s="6"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="49" t="s">
+      <c r="A24" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="B24" s="50" t="s">
+      <c r="B24" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="51" t="s">
+      <c r="C24" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="45"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="62"/>
+      <c r="G24" s="64"/>
       <c r="H24" s="6"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="52" t="s">
+      <c r="A25" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="53" t="s">
+      <c r="B25" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="54" t="s">
+      <c r="C25" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="43" t="s">
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="61" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="55" t="s">
+      <c r="A26" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="56" t="s">
+      <c r="B26" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="57" t="s">
+      <c r="C26" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="44"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="66"/>
+      <c r="F26" s="66"/>
+      <c r="G26" s="66"/>
+      <c r="H26" s="65"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
@@ -2049,7 +2137,7 @@
       <c r="A30" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B30" s="32" t="s">
+      <c r="B30" s="55" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2057,7 +2145,7 @@
       <c r="A31" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B31" s="34"/>
+      <c r="B31" s="56"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
@@ -2069,6 +2157,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="A8:A9"/>
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="D20:H20"/>
     <mergeCell ref="E21:H21"/>
@@ -2081,13 +2176,611 @@
     <mergeCell ref="G23:G25"/>
     <mergeCell ref="H25:H26"/>
     <mergeCell ref="D26:G26"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="32" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="63" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="67"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="63" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="67"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="72" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="72" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="72" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="72" t="s">
+        <v>90</v>
+      </c>
+      <c r="G5" s="72" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="72" t="s">
+        <v>91</v>
+      </c>
+      <c r="I5" s="72" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="73" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="67"/>
+      <c r="B7" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="J7" s="27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="63" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="68" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="53" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="53" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="53" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="54" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="67"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="I9" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="67"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="51" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="51" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="I10" s="51" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="52" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="62"/>
+      <c r="B11" s="66"/>
+      <c r="C11" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="69" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" s="70" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="70" t="s">
+        <v>97</v>
+      </c>
+      <c r="E12" s="70" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="70" t="s">
+        <v>98</v>
+      </c>
+      <c r="G12" s="70" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="70" t="s">
+        <v>99</v>
+      </c>
+      <c r="I12" s="70" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="71" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="47" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="44" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="57" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="58"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="13"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="59"/>
+      <c r="H19" s="60"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" s="13"/>
+      <c r="E20" s="61" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" s="59"/>
+      <c r="G20" s="59"/>
+      <c r="H20" s="60"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="13"/>
+      <c r="E21" s="65"/>
+      <c r="F21" s="63" t="s">
+        <v>76</v>
+      </c>
+      <c r="G21" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="H21" s="30"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="59"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="64"/>
+      <c r="H22" s="30"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="47" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" s="59"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="61" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="50" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="66"/>
+      <c r="E24" s="66"/>
+      <c r="F24" s="66"/>
+      <c r="G24" s="66"/>
+      <c r="H24" s="65"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="32" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" s="55" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="56"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="32" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="D24:G24"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="D18:H18"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="H23:H24"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="B8:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>